<commit_message>
uploaded the new dataset
new dataset contains all the articles in whole
</commit_message>
<xml_diff>
--- a/Documentation/499a.xlsx
+++ b/Documentation/499a.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="1099">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="1099">
   <si>
     <t>Genre</t>
   </si>
@@ -4480,8 +4480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K90"/>
   <sheetViews>
-    <sheetView zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView topLeftCell="A90" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6125,8 +6125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView topLeftCell="B65" zoomScale="84" workbookViewId="0">
-      <selection activeCell="H68" sqref="H68"/>
+    <sheetView topLeftCell="B66" zoomScale="84" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7335,12 +7335,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F125" sqref="F125"/>
+    <sheetView tabSelected="1" topLeftCell="A164" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B168" sqref="B168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="2" max="2" width="19.54296875" customWidth="1"/>
     <col min="5" max="5" width="16.7265625" customWidth="1"/>
     <col min="6" max="6" width="31.81640625" customWidth="1"/>
     <col min="7" max="7" width="21.81640625" customWidth="1"/>

</xml_diff>